<commit_message>
导入nuget for unity 插件
</commit_message>
<xml_diff>
--- a/Excel/测试用配置.xlsx
+++ b/Excel/测试用配置.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHubProject\MyGame\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{394F4F87-FE31-40AA-83B7-A9A154EFA481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9727326-9105-491B-9884-E85065B6B5E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>TestConfig</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -56,10 +56,6 @@
   </si>
   <si>
     <t>名字</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>String</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -401,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -441,10 +437,10 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -452,20 +448,20 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>5</v>
+      <c r="A6">
+        <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -473,7 +469,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -481,18 +477,10 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>4</v>
-      </c>
-      <c r="B10" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>